<commit_message>
added first round of data
</commit_message>
<xml_diff>
--- a/TLPR21_Raw_Master.xlsx
+++ b/TLPR21_Raw_Master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tayrlindsay/Desktop/GITHUB/TLPR21/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDE6564-9E6B-254C-AA7B-D66F073DFF2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B2C2E7-239E-5F4F-8AF2-91444DF5B5DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8940" yWindow="500" windowWidth="20840" windowHeight="13840" xr2:uid="{9F99DBB5-C4DA-A948-85BF-A7F1A69C1BCE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13840" xr2:uid="{9F99DBB5-C4DA-A948-85BF-A7F1A69C1BCE}"/>
   </bookViews>
   <sheets>
     <sheet name="RAW" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1255" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1457" uniqueCount="370">
   <si>
     <t>Species</t>
   </si>
@@ -1139,7 +1139,13 @@
     <t>Colony_Number</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>HLE</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>L</t>
   </si>
 </sst>
 </file>
@@ -1662,8 +1668,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFED04EC-AF48-A04F-A9D1-211D7C4EE961}">
   <dimension ref="A1:V833"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A274" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F276" sqref="F276"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="L1" sqref="L1"/>
+      <selection pane="bottomLeft" activeCell="N134" sqref="N134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1677,7 +1685,7 @@
     <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.33203125" customWidth="1"/>
-    <col min="10" max="10" width="5.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="12.5" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
@@ -6223,11 +6231,44 @@
         <v>43</v>
       </c>
       <c r="J128" s="29"/>
-      <c r="K128" s="7"/>
-      <c r="N128" s="7"/>
-      <c r="U128" s="7"/>
-    </row>
-    <row r="129" spans="1:21">
+      <c r="K128" s="7">
+        <v>44760</v>
+      </c>
+      <c r="L128" s="1">
+        <v>22</v>
+      </c>
+      <c r="M128" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N128" s="7">
+        <v>44760</v>
+      </c>
+      <c r="O128" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P128" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q128" s="1">
+        <v>14</v>
+      </c>
+      <c r="R128" s="1">
+        <v>15</v>
+      </c>
+      <c r="S128" s="1">
+        <v>16</v>
+      </c>
+      <c r="T128" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="U128" s="7">
+        <v>44761</v>
+      </c>
+      <c r="V128" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="129" spans="1:22">
       <c r="A129" s="17">
         <v>144</v>
       </c>
@@ -6256,11 +6297,44 @@
         <v>43</v>
       </c>
       <c r="J129" s="6"/>
-      <c r="K129" s="7"/>
-      <c r="N129" s="7"/>
-      <c r="U129" s="7"/>
-    </row>
-    <row r="130" spans="1:21">
+      <c r="K129" s="7">
+        <v>44760</v>
+      </c>
+      <c r="L129" s="1">
+        <v>26.5</v>
+      </c>
+      <c r="M129" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N129" s="7">
+        <v>44760</v>
+      </c>
+      <c r="O129" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P129" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q129" s="1">
+        <v>14</v>
+      </c>
+      <c r="R129" s="1">
+        <v>15</v>
+      </c>
+      <c r="S129" s="1">
+        <v>16</v>
+      </c>
+      <c r="T129" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="U129" s="7">
+        <v>44761</v>
+      </c>
+      <c r="V129" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="130" spans="1:22">
       <c r="A130" s="17">
         <v>145</v>
       </c>
@@ -6289,11 +6363,44 @@
         <v>43</v>
       </c>
       <c r="J130" s="6"/>
-      <c r="K130" s="7"/>
-      <c r="N130" s="7"/>
-      <c r="U130" s="7"/>
-    </row>
-    <row r="131" spans="1:21">
+      <c r="K130" s="7">
+        <v>44760</v>
+      </c>
+      <c r="L130" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="M130" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N130" s="7">
+        <v>44760</v>
+      </c>
+      <c r="O130" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="P130" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q130" s="1">
+        <v>14</v>
+      </c>
+      <c r="R130" s="1">
+        <v>15</v>
+      </c>
+      <c r="S130" s="1">
+        <v>16</v>
+      </c>
+      <c r="T130" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="U130" s="7">
+        <v>44761</v>
+      </c>
+      <c r="V130" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="131" spans="1:22">
       <c r="A131" s="17">
         <v>148</v>
       </c>
@@ -6322,11 +6429,44 @@
         <v>43</v>
       </c>
       <c r="J131" s="6"/>
-      <c r="K131" s="7"/>
-      <c r="N131" s="7"/>
-      <c r="U131" s="7"/>
-    </row>
-    <row r="132" spans="1:21">
+      <c r="K131" s="7">
+        <v>44760</v>
+      </c>
+      <c r="L131" s="1">
+        <v>9</v>
+      </c>
+      <c r="M131" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N131" s="7">
+        <v>44760</v>
+      </c>
+      <c r="O131" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P131" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q131" s="1">
+        <v>14</v>
+      </c>
+      <c r="R131" s="1">
+        <v>15</v>
+      </c>
+      <c r="S131" s="1">
+        <v>16</v>
+      </c>
+      <c r="T131" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="U131" s="7">
+        <v>44761</v>
+      </c>
+      <c r="V131" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="132" spans="1:22">
       <c r="A132" s="17">
         <v>150</v>
       </c>
@@ -6355,11 +6495,44 @@
         <v>43</v>
       </c>
       <c r="J132" s="6"/>
-      <c r="K132" s="7"/>
-      <c r="N132" s="7"/>
-      <c r="U132" s="7"/>
-    </row>
-    <row r="133" spans="1:21">
+      <c r="K132" s="7">
+        <v>44760</v>
+      </c>
+      <c r="L132" s="1">
+        <v>18</v>
+      </c>
+      <c r="M132" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N132" s="7">
+        <v>44760</v>
+      </c>
+      <c r="O132" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P132" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q132" s="1">
+        <v>14</v>
+      </c>
+      <c r="R132" s="1">
+        <v>15</v>
+      </c>
+      <c r="S132" s="1">
+        <v>16</v>
+      </c>
+      <c r="T132" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="U132" s="7">
+        <v>44761</v>
+      </c>
+      <c r="V132" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="133" spans="1:22">
       <c r="A133" s="17">
         <v>156</v>
       </c>
@@ -6388,11 +6561,44 @@
         <v>43</v>
       </c>
       <c r="J133" s="6"/>
-      <c r="K133" s="7"/>
-      <c r="N133" s="7"/>
-      <c r="U133" s="7"/>
-    </row>
-    <row r="134" spans="1:21">
+      <c r="K133" s="7">
+        <v>44760</v>
+      </c>
+      <c r="L133" s="1">
+        <v>16.5</v>
+      </c>
+      <c r="M133" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N133" s="7">
+        <v>44760</v>
+      </c>
+      <c r="O133" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P133" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q133" s="1">
+        <v>14</v>
+      </c>
+      <c r="R133" s="1">
+        <v>15</v>
+      </c>
+      <c r="S133" s="1">
+        <v>16</v>
+      </c>
+      <c r="T133" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="U133" s="7">
+        <v>44761</v>
+      </c>
+      <c r="V133" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="134" spans="1:22">
       <c r="A134" s="13">
         <v>328</v>
       </c>
@@ -6421,11 +6627,44 @@
         <v>43</v>
       </c>
       <c r="J134" s="6"/>
-      <c r="K134" s="7"/>
-      <c r="N134" s="7"/>
-      <c r="U134" s="7"/>
-    </row>
-    <row r="135" spans="1:21">
+      <c r="K134" s="7">
+        <v>44760</v>
+      </c>
+      <c r="L134" s="1">
+        <v>17.5</v>
+      </c>
+      <c r="M134" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N134" s="7">
+        <v>44760</v>
+      </c>
+      <c r="O134" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P134" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q134" s="1">
+        <v>14</v>
+      </c>
+      <c r="R134" s="1">
+        <v>15</v>
+      </c>
+      <c r="S134" s="1">
+        <v>16</v>
+      </c>
+      <c r="T134" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="U134" s="7">
+        <v>44761</v>
+      </c>
+      <c r="V134" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="135" spans="1:22">
       <c r="A135" s="13">
         <v>329</v>
       </c>
@@ -6454,11 +6693,44 @@
         <v>43</v>
       </c>
       <c r="J135" s="6"/>
-      <c r="K135" s="7"/>
-      <c r="N135" s="7"/>
-      <c r="U135" s="7"/>
-    </row>
-    <row r="136" spans="1:21">
+      <c r="K135" s="7">
+        <v>44760</v>
+      </c>
+      <c r="L135" s="1">
+        <v>16.5</v>
+      </c>
+      <c r="M135" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N135" s="7">
+        <v>44760</v>
+      </c>
+      <c r="O135" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="P135" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q135" s="1">
+        <v>14</v>
+      </c>
+      <c r="R135" s="1">
+        <v>15</v>
+      </c>
+      <c r="S135" s="1">
+        <v>16</v>
+      </c>
+      <c r="T135" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="U135" s="7">
+        <v>44761</v>
+      </c>
+      <c r="V135" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="136" spans="1:22">
       <c r="A136" s="13">
         <v>330</v>
       </c>
@@ -6487,11 +6759,44 @@
         <v>43</v>
       </c>
       <c r="J136" s="6"/>
-      <c r="K136" s="7"/>
-      <c r="N136" s="7"/>
-      <c r="U136" s="7"/>
-    </row>
-    <row r="137" spans="1:21">
+      <c r="K136" s="7">
+        <v>44760</v>
+      </c>
+      <c r="L136" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="M136" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N136" s="7">
+        <v>44760</v>
+      </c>
+      <c r="O136" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P136" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q136" s="1">
+        <v>14</v>
+      </c>
+      <c r="R136" s="1">
+        <v>15</v>
+      </c>
+      <c r="S136" s="1">
+        <v>16</v>
+      </c>
+      <c r="T136" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="U136" s="7">
+        <v>44761</v>
+      </c>
+      <c r="V136" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="137" spans="1:22">
       <c r="A137" s="13">
         <v>331</v>
       </c>
@@ -6520,11 +6825,44 @@
         <v>43</v>
       </c>
       <c r="J137" s="6"/>
-      <c r="K137" s="7"/>
-      <c r="N137" s="7"/>
-      <c r="U137" s="7"/>
-    </row>
-    <row r="138" spans="1:21">
+      <c r="K137" s="7">
+        <v>44760</v>
+      </c>
+      <c r="L137" s="1">
+        <v>14.5</v>
+      </c>
+      <c r="M137" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N137" s="7">
+        <v>44760</v>
+      </c>
+      <c r="O137" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="P137" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q137" s="1">
+        <v>14</v>
+      </c>
+      <c r="R137" s="1">
+        <v>15</v>
+      </c>
+      <c r="S137" s="1">
+        <v>16</v>
+      </c>
+      <c r="T137" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="U137" s="7">
+        <v>44761</v>
+      </c>
+      <c r="V137" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="138" spans="1:22">
       <c r="A138" s="13">
         <v>333</v>
       </c>
@@ -6552,9 +6890,44 @@
       <c r="I138" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="K138" s="7"/>
-    </row>
-    <row r="139" spans="1:21">
+      <c r="K138" s="7">
+        <v>44760</v>
+      </c>
+      <c r="L138" s="1">
+        <v>17.5</v>
+      </c>
+      <c r="M138" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N138" s="7">
+        <v>44760</v>
+      </c>
+      <c r="O138" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P138" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q138" s="1">
+        <v>14</v>
+      </c>
+      <c r="R138" s="1">
+        <v>15</v>
+      </c>
+      <c r="S138" s="1">
+        <v>16</v>
+      </c>
+      <c r="T138" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="U138" s="7">
+        <v>44761</v>
+      </c>
+      <c r="V138" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="139" spans="1:22">
       <c r="A139" s="13">
         <v>338</v>
       </c>
@@ -6582,11 +6955,44 @@
       <c r="I139" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="K139" s="7"/>
-      <c r="L139" s="9"/>
-      <c r="N139" s="7"/>
-    </row>
-    <row r="140" spans="1:21">
+      <c r="K139" s="7">
+        <v>44760</v>
+      </c>
+      <c r="L139" s="1">
+        <v>19.5</v>
+      </c>
+      <c r="M139" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N139" s="7">
+        <v>44760</v>
+      </c>
+      <c r="O139" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P139" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q139" s="1">
+        <v>14</v>
+      </c>
+      <c r="R139" s="1">
+        <v>15</v>
+      </c>
+      <c r="S139" s="1">
+        <v>16</v>
+      </c>
+      <c r="T139" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="U139" s="7">
+        <v>44761</v>
+      </c>
+      <c r="V139" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="140" spans="1:22">
       <c r="A140" s="13">
         <v>343</v>
       </c>
@@ -6614,10 +7020,45 @@
       <c r="I140" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="K140" s="7"/>
-      <c r="L140" s="9"/>
-    </row>
-    <row r="141" spans="1:21">
+      <c r="J140" s="7"/>
+      <c r="K140" s="7">
+        <v>44720</v>
+      </c>
+      <c r="L140" s="1">
+        <v>27.5</v>
+      </c>
+      <c r="M140" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N140" s="7">
+        <v>44760</v>
+      </c>
+      <c r="O140" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P140" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q140" s="1">
+        <v>14</v>
+      </c>
+      <c r="R140" s="1">
+        <v>15</v>
+      </c>
+      <c r="S140" s="1">
+        <v>16</v>
+      </c>
+      <c r="T140" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="U140" s="7">
+        <v>44761</v>
+      </c>
+      <c r="V140" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="141" spans="1:22">
       <c r="A141" s="13">
         <v>350</v>
       </c>
@@ -6645,11 +7086,45 @@
       <c r="I141" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="K141" s="7"/>
-      <c r="L141" s="9"/>
-      <c r="N141" s="7"/>
-    </row>
-    <row r="142" spans="1:21">
+      <c r="J141" s="7"/>
+      <c r="K141" s="7">
+        <v>44720</v>
+      </c>
+      <c r="L141" s="1">
+        <v>40.5</v>
+      </c>
+      <c r="M141" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N141" s="7">
+        <v>44760</v>
+      </c>
+      <c r="O141" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P141" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q141" s="1">
+        <v>14</v>
+      </c>
+      <c r="R141" s="1">
+        <v>15</v>
+      </c>
+      <c r="S141" s="1">
+        <v>16</v>
+      </c>
+      <c r="T141" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="U141" s="7">
+        <v>44761</v>
+      </c>
+      <c r="V141" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="142" spans="1:22">
       <c r="A142" s="13">
         <v>363</v>
       </c>
@@ -6677,10 +7152,44 @@
       <c r="I142" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="K142" s="7"/>
-      <c r="L142" s="9"/>
-    </row>
-    <row r="143" spans="1:21">
+      <c r="K142" s="7">
+        <v>44760</v>
+      </c>
+      <c r="L142" s="1">
+        <v>23</v>
+      </c>
+      <c r="M142" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N142" s="7">
+        <v>44760</v>
+      </c>
+      <c r="O142" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P142" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q142" s="1">
+        <v>14</v>
+      </c>
+      <c r="R142" s="1">
+        <v>15</v>
+      </c>
+      <c r="S142" s="1">
+        <v>16</v>
+      </c>
+      <c r="T142" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="U142" s="7">
+        <v>44761</v>
+      </c>
+      <c r="V142" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="143" spans="1:22">
       <c r="A143" s="13">
         <v>366</v>
       </c>
@@ -6708,11 +7217,45 @@
       <c r="I143" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="K143" s="7"/>
-      <c r="L143" s="9"/>
-      <c r="N143" s="7"/>
-    </row>
-    <row r="144" spans="1:21">
+      <c r="J143" s="7"/>
+      <c r="K143" s="7">
+        <v>44720</v>
+      </c>
+      <c r="L143" s="1">
+        <v>38.5</v>
+      </c>
+      <c r="M143" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N143" s="7">
+        <v>44760</v>
+      </c>
+      <c r="O143" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P143" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q143" s="1">
+        <v>14</v>
+      </c>
+      <c r="R143" s="1">
+        <v>15</v>
+      </c>
+      <c r="S143" s="1">
+        <v>16</v>
+      </c>
+      <c r="T143" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="U143" s="7">
+        <v>44761</v>
+      </c>
+      <c r="V143" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="144" spans="1:22">
       <c r="A144" s="17">
         <v>161</v>
       </c>
@@ -6740,12 +7283,43 @@
       <c r="I144" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="J144" s="6"/>
-      <c r="K144" s="7" t="s">
+      <c r="J144" s="7"/>
+      <c r="K144" s="7">
+        <v>44720</v>
+      </c>
+      <c r="L144" s="1">
+        <v>28</v>
+      </c>
+      <c r="M144" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N144" s="7">
+        <v>44760</v>
+      </c>
+      <c r="O144" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P144" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q144" s="1">
+        <v>14</v>
+      </c>
+      <c r="R144" s="1">
+        <v>15</v>
+      </c>
+      <c r="S144" s="1">
+        <v>16</v>
+      </c>
+      <c r="T144" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="U144" s="7">
+        <v>44761</v>
+      </c>
+      <c r="V144" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="N144" s="7"/>
-      <c r="U144" s="7"/>
     </row>
     <row r="145" spans="1:22">
       <c r="A145" s="17">
@@ -6776,9 +7350,42 @@
         <v>43</v>
       </c>
       <c r="J145" s="6"/>
-      <c r="K145" s="7"/>
-      <c r="N145" s="7"/>
-      <c r="U145" s="7"/>
+      <c r="K145" s="7">
+        <v>44760</v>
+      </c>
+      <c r="L145" s="1">
+        <v>23</v>
+      </c>
+      <c r="M145" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N145" s="7">
+        <v>44760</v>
+      </c>
+      <c r="O145" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P145" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q145" s="1">
+        <v>14</v>
+      </c>
+      <c r="R145" s="1">
+        <v>15</v>
+      </c>
+      <c r="S145" s="1">
+        <v>16</v>
+      </c>
+      <c r="T145" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="U145" s="7">
+        <v>44761</v>
+      </c>
+      <c r="V145" s="1" t="s">
+        <v>367</v>
+      </c>
     </row>
     <row r="146" spans="1:22">
       <c r="A146" s="17">
@@ -6809,18 +7416,42 @@
         <v>43</v>
       </c>
       <c r="J146" s="6"/>
-      <c r="K146" s="6"/>
-      <c r="L146" s="6"/>
-      <c r="M146" s="6"/>
-      <c r="N146" s="6"/>
-      <c r="O146" s="6"/>
-      <c r="P146" s="6"/>
-      <c r="Q146" s="6"/>
-      <c r="R146" s="6"/>
-      <c r="S146" s="6"/>
-      <c r="T146" s="6"/>
-      <c r="U146" s="6"/>
-      <c r="V146" s="6"/>
+      <c r="K146" s="7">
+        <v>44760</v>
+      </c>
+      <c r="L146" s="1">
+        <v>17</v>
+      </c>
+      <c r="M146" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N146" s="7">
+        <v>44760</v>
+      </c>
+      <c r="O146" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P146" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q146" s="1">
+        <v>14</v>
+      </c>
+      <c r="R146" s="1">
+        <v>15</v>
+      </c>
+      <c r="S146" s="1">
+        <v>16</v>
+      </c>
+      <c r="T146" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="U146" s="7">
+        <v>44761</v>
+      </c>
+      <c r="V146" s="1" t="s">
+        <v>367</v>
+      </c>
     </row>
     <row r="147" spans="1:22">
       <c r="A147" s="17">
@@ -6851,9 +7482,42 @@
         <v>43</v>
       </c>
       <c r="J147" s="6"/>
-      <c r="K147" s="7"/>
-      <c r="N147" s="7"/>
-      <c r="U147" s="7"/>
+      <c r="K147" s="7">
+        <v>44760</v>
+      </c>
+      <c r="L147" s="1">
+        <v>26.5</v>
+      </c>
+      <c r="M147" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N147" s="7">
+        <v>44760</v>
+      </c>
+      <c r="O147" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P147" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q147" s="1">
+        <v>14</v>
+      </c>
+      <c r="R147" s="1">
+        <v>15</v>
+      </c>
+      <c r="S147" s="1">
+        <v>16</v>
+      </c>
+      <c r="T147" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="U147" s="7">
+        <v>44761</v>
+      </c>
+      <c r="V147" s="1" t="s">
+        <v>367</v>
+      </c>
     </row>
     <row r="148" spans="1:22">
       <c r="A148" s="17">
@@ -6884,9 +7548,42 @@
         <v>43</v>
       </c>
       <c r="J148" s="6"/>
-      <c r="K148" s="7"/>
-      <c r="N148" s="7"/>
-      <c r="U148" s="7"/>
+      <c r="K148" s="7">
+        <v>44760</v>
+      </c>
+      <c r="L148" s="1">
+        <v>14.5</v>
+      </c>
+      <c r="M148" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N148" s="7">
+        <v>44760</v>
+      </c>
+      <c r="O148" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="P148" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q148" s="1">
+        <v>14</v>
+      </c>
+      <c r="R148" s="1">
+        <v>15</v>
+      </c>
+      <c r="S148" s="1">
+        <v>16</v>
+      </c>
+      <c r="T148" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="U148" s="7">
+        <v>44761</v>
+      </c>
+      <c r="V148" s="1" t="s">
+        <v>367</v>
+      </c>
     </row>
     <row r="149" spans="1:22">
       <c r="A149" s="15">
@@ -6916,6 +7613,45 @@
       <c r="I149" s="19" t="s">
         <v>43</v>
       </c>
+      <c r="J149" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K149" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L149" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M149" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N149" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O149" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P149" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q149" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="R149" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S149" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="T149" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="U149" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V149" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="150" spans="1:22">
       <c r="A150" s="15">
@@ -6945,6 +7681,45 @@
       <c r="I150" s="19" t="s">
         <v>43</v>
       </c>
+      <c r="J150" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K150" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L150" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M150" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N150" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O150" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P150" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q150" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="R150" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S150" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="T150" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="U150" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V150" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="151" spans="1:22">
       <c r="A151" s="15">
@@ -6974,6 +7749,43 @@
       <c r="I151" s="19" t="s">
         <v>43</v>
       </c>
+      <c r="J151" s="7"/>
+      <c r="K151" s="7">
+        <v>44761</v>
+      </c>
+      <c r="L151" s="1">
+        <v>19.5</v>
+      </c>
+      <c r="M151" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N151" s="7">
+        <v>44761</v>
+      </c>
+      <c r="O151" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="P151" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q151" s="1">
+        <v>14</v>
+      </c>
+      <c r="R151" s="1">
+        <v>15</v>
+      </c>
+      <c r="S151" s="1">
+        <v>16</v>
+      </c>
+      <c r="T151" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="U151" s="7">
+        <v>44769</v>
+      </c>
+      <c r="V151" s="1" t="s">
+        <v>367</v>
+      </c>
     </row>
     <row r="152" spans="1:22">
       <c r="A152" s="15">
@@ -7003,6 +7815,45 @@
       <c r="I152" s="19" t="s">
         <v>43</v>
       </c>
+      <c r="J152" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K152" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L152" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M152" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N152" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O152" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P152" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q152" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="R152" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S152" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="T152" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="U152" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V152" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="153" spans="1:22">
       <c r="A153" s="15">
@@ -7032,6 +7883,42 @@
       <c r="I153" s="19" t="s">
         <v>43</v>
       </c>
+      <c r="K153" s="7">
+        <v>44761</v>
+      </c>
+      <c r="L153" s="1">
+        <v>22</v>
+      </c>
+      <c r="M153" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N153" s="7">
+        <v>44761</v>
+      </c>
+      <c r="O153" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="P153" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q153" s="1">
+        <v>14</v>
+      </c>
+      <c r="R153" s="1">
+        <v>15</v>
+      </c>
+      <c r="S153" s="1">
+        <v>16</v>
+      </c>
+      <c r="T153" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="U153" s="7">
+        <v>44769</v>
+      </c>
+      <c r="V153" s="1" t="s">
+        <v>367</v>
+      </c>
     </row>
     <row r="154" spans="1:22">
       <c r="A154" s="15">
@@ -7061,6 +7948,42 @@
       <c r="I154" s="19" t="s">
         <v>43</v>
       </c>
+      <c r="K154" s="7">
+        <v>44767</v>
+      </c>
+      <c r="L154" s="1">
+        <v>15</v>
+      </c>
+      <c r="M154" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N154" s="7">
+        <v>44767</v>
+      </c>
+      <c r="O154" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="P154" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q154" s="1">
+        <v>14</v>
+      </c>
+      <c r="R154" s="1">
+        <v>15</v>
+      </c>
+      <c r="S154" s="1">
+        <v>16</v>
+      </c>
+      <c r="T154" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="U154" s="7">
+        <v>44769</v>
+      </c>
+      <c r="V154" s="1" t="s">
+        <v>367</v>
+      </c>
     </row>
     <row r="155" spans="1:22">
       <c r="A155" s="15">
@@ -7090,6 +8013,42 @@
       <c r="I155" s="19" t="s">
         <v>43</v>
       </c>
+      <c r="K155" s="7">
+        <v>44762</v>
+      </c>
+      <c r="L155" s="1">
+        <v>17.5</v>
+      </c>
+      <c r="M155" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N155" s="7">
+        <v>44762</v>
+      </c>
+      <c r="O155" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="P155" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q155" s="1">
+        <v>14</v>
+      </c>
+      <c r="R155" s="1">
+        <v>15</v>
+      </c>
+      <c r="S155" s="1">
+        <v>16</v>
+      </c>
+      <c r="T155" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="U155" s="7">
+        <v>44769</v>
+      </c>
+      <c r="V155" s="1" t="s">
+        <v>367</v>
+      </c>
     </row>
     <row r="156" spans="1:22">
       <c r="A156" s="15" t="s">
@@ -7119,6 +8078,42 @@
       <c r="I156" s="19" t="s">
         <v>43</v>
       </c>
+      <c r="K156" s="7">
+        <v>44761</v>
+      </c>
+      <c r="L156" s="1">
+        <v>25.5</v>
+      </c>
+      <c r="M156" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N156" s="7">
+        <v>44761</v>
+      </c>
+      <c r="O156" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="P156" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q156" s="1">
+        <v>14</v>
+      </c>
+      <c r="R156" s="1">
+        <v>15</v>
+      </c>
+      <c r="S156" s="1">
+        <v>16</v>
+      </c>
+      <c r="T156" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="U156" s="7">
+        <v>44769</v>
+      </c>
+      <c r="V156" s="1" t="s">
+        <v>367</v>
+      </c>
     </row>
     <row r="157" spans="1:22">
       <c r="A157" s="15" t="s">
@@ -7148,6 +8143,42 @@
       <c r="I157" s="19" t="s">
         <v>43</v>
       </c>
+      <c r="K157" s="7">
+        <v>44761</v>
+      </c>
+      <c r="L157" s="1">
+        <v>28</v>
+      </c>
+      <c r="M157" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N157" s="7">
+        <v>44761</v>
+      </c>
+      <c r="O157" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="P157" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q157" s="1">
+        <v>14</v>
+      </c>
+      <c r="R157" s="1">
+        <v>15</v>
+      </c>
+      <c r="S157" s="1">
+        <v>16</v>
+      </c>
+      <c r="T157" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="U157" s="7">
+        <v>44769</v>
+      </c>
+      <c r="V157" s="1" t="s">
+        <v>367</v>
+      </c>
     </row>
     <row r="158" spans="1:22">
       <c r="A158" s="15">
@@ -7177,6 +8208,42 @@
       <c r="I158" s="19" t="s">
         <v>43</v>
       </c>
+      <c r="K158" s="7">
+        <v>44761</v>
+      </c>
+      <c r="L158" s="1">
+        <v>37</v>
+      </c>
+      <c r="M158" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N158" s="7">
+        <v>44761</v>
+      </c>
+      <c r="O158" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="P158" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q158" s="1">
+        <v>14</v>
+      </c>
+      <c r="R158" s="1">
+        <v>15</v>
+      </c>
+      <c r="S158" s="1">
+        <v>16</v>
+      </c>
+      <c r="T158" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="U158" s="7">
+        <v>44769</v>
+      </c>
+      <c r="V158" s="1" t="s">
+        <v>367</v>
+      </c>
     </row>
     <row r="159" spans="1:22">
       <c r="A159" s="15">
@@ -7206,6 +8273,42 @@
       <c r="I159" s="19" t="s">
         <v>43</v>
       </c>
+      <c r="K159" s="7">
+        <v>44761</v>
+      </c>
+      <c r="L159" s="1">
+        <v>17.5</v>
+      </c>
+      <c r="M159" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N159" s="7">
+        <v>44761</v>
+      </c>
+      <c r="O159" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="P159" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q159" s="1">
+        <v>14</v>
+      </c>
+      <c r="R159" s="1">
+        <v>15</v>
+      </c>
+      <c r="S159" s="1">
+        <v>16</v>
+      </c>
+      <c r="T159" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="U159" s="7">
+        <v>44769</v>
+      </c>
+      <c r="V159" s="1" t="s">
+        <v>367</v>
+      </c>
     </row>
     <row r="160" spans="1:22">
       <c r="A160" s="15">
@@ -7235,8 +8338,44 @@
       <c r="I160" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="161" spans="1:9">
+      <c r="K160" s="7">
+        <v>44761</v>
+      </c>
+      <c r="L160" s="1">
+        <v>25.5</v>
+      </c>
+      <c r="M160" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N160" s="7">
+        <v>44761</v>
+      </c>
+      <c r="O160" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="P160" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q160" s="1">
+        <v>14</v>
+      </c>
+      <c r="R160" s="1">
+        <v>15</v>
+      </c>
+      <c r="S160" s="1">
+        <v>16</v>
+      </c>
+      <c r="T160" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="U160" s="7">
+        <v>44769</v>
+      </c>
+      <c r="V160" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="161" spans="1:22">
       <c r="A161" s="15">
         <v>24</v>
       </c>
@@ -7264,8 +8403,44 @@
       <c r="I161" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="162" spans="1:9">
+      <c r="K161" s="7">
+        <v>44767</v>
+      </c>
+      <c r="L161" s="1">
+        <v>19</v>
+      </c>
+      <c r="M161" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N161" s="7">
+        <v>44767</v>
+      </c>
+      <c r="O161" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="P161" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q161" s="1">
+        <v>14</v>
+      </c>
+      <c r="R161" s="1">
+        <v>15</v>
+      </c>
+      <c r="S161" s="1">
+        <v>16</v>
+      </c>
+      <c r="T161" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="U161" s="7">
+        <v>44769</v>
+      </c>
+      <c r="V161" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="162" spans="1:22">
       <c r="A162" s="15">
         <v>29</v>
       </c>
@@ -7293,8 +8468,44 @@
       <c r="I162" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="163" spans="1:9">
+      <c r="K162" s="7">
+        <v>44761</v>
+      </c>
+      <c r="L162" s="1">
+        <v>20.5</v>
+      </c>
+      <c r="M162" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N162" s="7">
+        <v>44761</v>
+      </c>
+      <c r="O162" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="P162" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q162" s="1">
+        <v>14</v>
+      </c>
+      <c r="R162" s="1">
+        <v>15</v>
+      </c>
+      <c r="S162" s="1">
+        <v>16</v>
+      </c>
+      <c r="T162" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="U162" s="7">
+        <v>44769</v>
+      </c>
+      <c r="V162" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="163" spans="1:22">
       <c r="A163" s="15">
         <v>48</v>
       </c>
@@ -7322,8 +8533,44 @@
       <c r="I163" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="164" spans="1:9">
+      <c r="K163" s="7">
+        <v>44761</v>
+      </c>
+      <c r="L163" s="1">
+        <v>30.5</v>
+      </c>
+      <c r="M163" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N163" s="7">
+        <v>44761</v>
+      </c>
+      <c r="O163" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="P163" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q163" s="1">
+        <v>14</v>
+      </c>
+      <c r="R163" s="1">
+        <v>15</v>
+      </c>
+      <c r="S163" s="1">
+        <v>16</v>
+      </c>
+      <c r="T163" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="U163" s="7">
+        <v>44769</v>
+      </c>
+      <c r="V163" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="164" spans="1:22">
       <c r="A164" s="15">
         <v>52</v>
       </c>
@@ -7351,8 +8598,44 @@
       <c r="I164" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="165" spans="1:9">
+      <c r="K164" s="7">
+        <v>44767</v>
+      </c>
+      <c r="L164" s="1">
+        <v>20</v>
+      </c>
+      <c r="M164" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N164" s="7">
+        <v>44767</v>
+      </c>
+      <c r="O164" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="P164" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q164" s="1">
+        <v>14</v>
+      </c>
+      <c r="R164" s="1">
+        <v>15</v>
+      </c>
+      <c r="S164" s="1">
+        <v>16</v>
+      </c>
+      <c r="T164" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="U164" s="7">
+        <v>44769</v>
+      </c>
+      <c r="V164" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="165" spans="1:22">
       <c r="A165" s="15">
         <v>53</v>
       </c>
@@ -7380,8 +8663,44 @@
       <c r="I165" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="166" spans="1:9">
+      <c r="K165" s="7">
+        <v>44761</v>
+      </c>
+      <c r="L165" s="1">
+        <v>22</v>
+      </c>
+      <c r="M165" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N165" s="7">
+        <v>44761</v>
+      </c>
+      <c r="O165" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="P165" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q165" s="1">
+        <v>14</v>
+      </c>
+      <c r="R165" s="1">
+        <v>15</v>
+      </c>
+      <c r="S165" s="1">
+        <v>16</v>
+      </c>
+      <c r="T165" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="U165" s="7">
+        <v>44769</v>
+      </c>
+      <c r="V165" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="166" spans="1:22">
       <c r="A166" s="15">
         <v>54</v>
       </c>
@@ -7409,8 +8728,44 @@
       <c r="I166" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="167" spans="1:9">
+      <c r="K166" s="7">
+        <v>44761</v>
+      </c>
+      <c r="L166" s="1">
+        <v>35.5</v>
+      </c>
+      <c r="M166" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N166" s="7">
+        <v>44761</v>
+      </c>
+      <c r="O166" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="P166" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q166" s="1">
+        <v>14</v>
+      </c>
+      <c r="R166" s="1">
+        <v>15</v>
+      </c>
+      <c r="S166" s="1">
+        <v>16</v>
+      </c>
+      <c r="T166" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="U166" s="7">
+        <v>44769</v>
+      </c>
+      <c r="V166" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="167" spans="1:22">
       <c r="A167" s="15">
         <v>75</v>
       </c>
@@ -7438,8 +8793,44 @@
       <c r="I167" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="168" spans="1:9">
+      <c r="K167" s="7">
+        <v>44762</v>
+      </c>
+      <c r="L167" s="1">
+        <v>26.5</v>
+      </c>
+      <c r="M167" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N167" s="7">
+        <v>44762</v>
+      </c>
+      <c r="O167" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="P167" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q167" s="1">
+        <v>14</v>
+      </c>
+      <c r="R167" s="1">
+        <v>15</v>
+      </c>
+      <c r="S167" s="1">
+        <v>16</v>
+      </c>
+      <c r="T167" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="U167" s="7">
+        <v>44769</v>
+      </c>
+      <c r="V167" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="168" spans="1:22">
       <c r="A168" s="15">
         <v>85</v>
       </c>
@@ -7467,8 +8858,44 @@
       <c r="I168" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="169" spans="1:9">
+      <c r="K168" s="7">
+        <v>44767</v>
+      </c>
+      <c r="L168" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="M168" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N168" s="7">
+        <v>44767</v>
+      </c>
+      <c r="O168" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="P168" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q168" s="1">
+        <v>14</v>
+      </c>
+      <c r="R168" s="1">
+        <v>15</v>
+      </c>
+      <c r="S168" s="1">
+        <v>16</v>
+      </c>
+      <c r="T168" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="U168" s="7">
+        <v>44769</v>
+      </c>
+      <c r="V168" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="169" spans="1:22">
       <c r="A169" s="15">
         <v>103</v>
       </c>
@@ -7496,8 +8923,44 @@
       <c r="I169" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="170" spans="1:9">
+      <c r="K169" s="7">
+        <v>44762</v>
+      </c>
+      <c r="L169" s="1">
+        <v>30.5</v>
+      </c>
+      <c r="M169" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N169" s="7">
+        <v>44762</v>
+      </c>
+      <c r="O169" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="P169" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q169" s="1">
+        <v>14</v>
+      </c>
+      <c r="R169" s="1">
+        <v>15</v>
+      </c>
+      <c r="S169" s="1">
+        <v>16</v>
+      </c>
+      <c r="T169" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="U169" s="7">
+        <v>44769</v>
+      </c>
+      <c r="V169" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="170" spans="1:22">
       <c r="A170" s="15">
         <v>105</v>
       </c>
@@ -7525,8 +8988,44 @@
       <c r="I170" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="171" spans="1:9">
+      <c r="K170" s="7">
+        <v>44761</v>
+      </c>
+      <c r="L170" s="1">
+        <v>17.5</v>
+      </c>
+      <c r="M170" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N170" s="7">
+        <v>44761</v>
+      </c>
+      <c r="O170" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="P170" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q170" s="1">
+        <v>14</v>
+      </c>
+      <c r="R170" s="1">
+        <v>15</v>
+      </c>
+      <c r="S170" s="1">
+        <v>16</v>
+      </c>
+      <c r="T170" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="U170" s="7">
+        <v>44769</v>
+      </c>
+      <c r="V170" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="171" spans="1:22">
       <c r="A171" s="15">
         <v>106</v>
       </c>
@@ -7554,8 +9053,44 @@
       <c r="I171" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="172" spans="1:9">
+      <c r="K171" s="7">
+        <v>44767</v>
+      </c>
+      <c r="L171" s="1">
+        <v>20</v>
+      </c>
+      <c r="M171" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="N171" s="7">
+        <v>44767</v>
+      </c>
+      <c r="O171" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="P171" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q171" s="1">
+        <v>14</v>
+      </c>
+      <c r="R171" s="1">
+        <v>15</v>
+      </c>
+      <c r="S171" s="1">
+        <v>16</v>
+      </c>
+      <c r="T171" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="U171" s="7">
+        <v>44769</v>
+      </c>
+      <c r="V171" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="172" spans="1:22">
       <c r="A172" s="13">
         <v>307</v>
       </c>
@@ -7583,8 +9118,11 @@
       <c r="I172" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="173" spans="1:9">
+      <c r="K172" s="7"/>
+      <c r="N172" s="7"/>
+      <c r="U172" s="7"/>
+    </row>
+    <row r="173" spans="1:22">
       <c r="A173" s="13">
         <v>308</v>
       </c>
@@ -7612,8 +9150,10 @@
       <c r="I173" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="174" spans="1:9">
+      <c r="N173" s="7"/>
+      <c r="U173" s="7"/>
+    </row>
+    <row r="174" spans="1:22">
       <c r="A174" s="13">
         <v>310</v>
       </c>
@@ -7641,8 +9181,10 @@
       <c r="I174" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="175" spans="1:9">
+      <c r="N174" s="7"/>
+      <c r="U174" s="7"/>
+    </row>
+    <row r="175" spans="1:22">
       <c r="A175" s="13">
         <v>311</v>
       </c>
@@ -7670,8 +9212,10 @@
       <c r="I175" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="176" spans="1:9">
+      <c r="N175" s="7"/>
+      <c r="U175" s="7"/>
+    </row>
+    <row r="176" spans="1:22">
       <c r="A176" s="13">
         <v>312</v>
       </c>
@@ -7699,8 +9243,10 @@
       <c r="I176" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="177" spans="1:9">
+      <c r="N176" s="7"/>
+      <c r="U176" s="7"/>
+    </row>
+    <row r="177" spans="1:21">
       <c r="A177" s="13">
         <v>313</v>
       </c>
@@ -7728,8 +9274,10 @@
       <c r="I177" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="178" spans="1:9">
+      <c r="N177" s="7"/>
+      <c r="U177" s="7"/>
+    </row>
+    <row r="178" spans="1:21">
       <c r="A178" s="13">
         <v>317</v>
       </c>
@@ -7757,8 +9305,10 @@
       <c r="I178" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="179" spans="1:9">
+      <c r="N178" s="7"/>
+      <c r="U178" s="7"/>
+    </row>
+    <row r="179" spans="1:21">
       <c r="A179" s="13">
         <v>213</v>
       </c>
@@ -7786,8 +9336,10 @@
       <c r="I179" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="180" spans="1:9">
+      <c r="N179" s="7"/>
+      <c r="U179" s="7"/>
+    </row>
+    <row r="180" spans="1:21">
       <c r="A180" s="13">
         <v>332</v>
       </c>
@@ -7815,8 +9367,10 @@
       <c r="I180" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="181" spans="1:9">
+      <c r="N180" s="7"/>
+      <c r="U180" s="7"/>
+    </row>
+    <row r="181" spans="1:21">
       <c r="A181" s="13">
         <v>334</v>
       </c>
@@ -7844,8 +9398,10 @@
       <c r="I181" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="182" spans="1:9">
+      <c r="N181" s="7"/>
+      <c r="U181" s="7"/>
+    </row>
+    <row r="182" spans="1:21">
       <c r="A182" s="13">
         <v>345</v>
       </c>
@@ -7873,8 +9429,10 @@
       <c r="I182" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="183" spans="1:9">
+      <c r="N182" s="7"/>
+      <c r="U182" s="7"/>
+    </row>
+    <row r="183" spans="1:21">
       <c r="A183" s="13">
         <v>347</v>
       </c>
@@ -7902,8 +9460,10 @@
       <c r="I183" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="184" spans="1:9">
+      <c r="N183" s="7"/>
+      <c r="U183" s="7"/>
+    </row>
+    <row r="184" spans="1:21">
       <c r="A184" s="13">
         <v>371</v>
       </c>
@@ -7931,8 +9491,10 @@
       <c r="I184" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="185" spans="1:9">
+      <c r="N184" s="7"/>
+      <c r="U184" s="7"/>
+    </row>
+    <row r="185" spans="1:21">
       <c r="A185" s="13">
         <v>372</v>
       </c>
@@ -7960,8 +9522,10 @@
       <c r="I185" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="186" spans="1:9">
+      <c r="N185" s="7"/>
+      <c r="U185" s="7"/>
+    </row>
+    <row r="186" spans="1:21">
       <c r="A186" s="36">
         <v>373</v>
       </c>
@@ -7989,8 +9553,10 @@
       <c r="I186" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="187" spans="1:9">
+      <c r="N186" s="7"/>
+      <c r="U186" s="7"/>
+    </row>
+    <row r="187" spans="1:21">
       <c r="A187" s="17">
         <v>170</v>
       </c>
@@ -8018,8 +9584,10 @@
       <c r="I187" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="188" spans="1:9">
+      <c r="N187" s="7"/>
+      <c r="U187" s="7"/>
+    </row>
+    <row r="188" spans="1:21">
       <c r="A188" s="17">
         <v>187</v>
       </c>
@@ -8047,8 +9615,10 @@
       <c r="I188" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="189" spans="1:9">
+      <c r="N188" s="7"/>
+      <c r="U188" s="7"/>
+    </row>
+    <row r="189" spans="1:21">
       <c r="A189" s="17">
         <v>189</v>
       </c>
@@ -8076,8 +9646,10 @@
       <c r="I189" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="190" spans="1:9">
+      <c r="N189" s="7"/>
+      <c r="U189" s="7"/>
+    </row>
+    <row r="190" spans="1:21">
       <c r="A190" s="17">
         <v>193</v>
       </c>
@@ -8105,8 +9677,10 @@
       <c r="I190" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="191" spans="1:9">
+      <c r="N190" s="7"/>
+      <c r="U190" s="7"/>
+    </row>
+    <row r="191" spans="1:21">
       <c r="A191" s="17">
         <v>194</v>
       </c>
@@ -8134,8 +9708,10 @@
       <c r="I191" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="192" spans="1:9">
+      <c r="N191" s="7"/>
+      <c r="U191" s="7"/>
+    </row>
+    <row r="192" spans="1:21">
       <c r="A192" s="15">
         <v>266</v>
       </c>

</xml_diff>